<commit_message>
introducing more readable differences and comapring names of sheets between files
</commit_message>
<xml_diff>
--- a/test_file_example_1.xlsx
+++ b/test_file_example_1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Python\compareXLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977D96AB-7242-402F-8C18-27B38CD2AFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE100C-8B6D-4EAD-987E-1F4F645D2E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="exceeding" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -406,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDE4FE7-774B-4F47-B5F4-87ED5A5FB65D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -425,4 +426,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940197CC-B382-4265-8C34-858F1C36B495}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change comparison text to match style
</commit_message>
<xml_diff>
--- a/test_file_example_1.xlsx
+++ b/test_file_example_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Python\compareXLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE100C-8B6D-4EAD-987E-1F4F645D2E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F8EC33-B067-41AB-94D7-78540567AFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -44,13 +44,13 @@
     <t>v2</t>
   </si>
   <si>
-    <t>vffff</t>
-  </si>
-  <si>
     <t>abeblio</t>
   </si>
   <si>
     <t>vvv</t>
+  </si>
+  <si>
+    <t>vfffff</t>
   </si>
 </sst>
 </file>
@@ -370,8 +370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +395,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -415,12 +415,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -432,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940197CC-B382-4265-8C34-858F1C36B495}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>